<commit_message>
Add BS and Github actions
</commit_message>
<xml_diff>
--- a/Manual_Test_Documents/Test Case Of UIKitCatalog.xlsx
+++ b/Manual_Test_Documents/Test Case Of UIKitCatalog.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="366">
   <si>
     <t>Project Name</t>
   </si>
@@ -778,7 +778,13 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Select</t>
+    <t>Verify Ok button will be enabled for valid alert message</t>
+  </si>
+  <si>
+    <t>Verify Ok button will not be enabled for an invalid alert message</t>
+  </si>
+  <si>
+    <t>Element Limitation</t>
   </si>
   <si>
     <t>Amader Rail</t>
@@ -858,6 +864,9 @@
 Phone: $#$#$%#%$&amp;
 Email: *^&amp;^&amp;^(^&amp;
 district: Tangail</t>
+  </si>
+  <si>
+    <t>Select</t>
   </si>
   <si>
     <t>Home Screen Section</t>
@@ -1835,7 +1844,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="145">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2211,6 +2220,9 @@
     <xf borderId="2" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="2" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="2" fillId="4" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
@@ -2248,7 +2260,7 @@
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="16">
     <dxf>
       <font>
         <b/>
@@ -2403,6 +2415,16 @@
       <font/>
       <fill>
         <patternFill patternType="none"/>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6FA8DC"/>
+          <bgColor rgb="FF6FA8DC"/>
+        </patternFill>
       </fill>
       <border/>
     </dxf>
@@ -8647,40 +8669,40 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="F32:F35"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="A19:J19"/>
-    <mergeCell ref="A21:J21"/>
-    <mergeCell ref="A23:J23"/>
-    <mergeCell ref="A26:J26"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="A36:J36"/>
-    <mergeCell ref="A40:J40"/>
-    <mergeCell ref="B37:B39"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="A7:J7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="F8:F9"/>
     <mergeCell ref="A10:J10"/>
+    <mergeCell ref="B11:B16"/>
+    <mergeCell ref="D11:D18"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="A19:J19"/>
+    <mergeCell ref="A21:J21"/>
+    <mergeCell ref="A23:J23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A26:J26"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="F37:F39"/>
+    <mergeCell ref="A40:J40"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="F41:F42"/>
     <mergeCell ref="A43:J43"/>
     <mergeCell ref="A45:J45"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B11:B16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="D11:D18"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="B32:B35"/>
     <mergeCell ref="D32:D35"/>
-    <mergeCell ref="F37:F39"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="F32:F35"/>
+    <mergeCell ref="A36:J36"/>
+    <mergeCell ref="B37:B39"/>
   </mergeCells>
   <conditionalFormatting sqref="J2">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
@@ -13582,7 +13604,7 @@
       </c>
       <c r="J2" s="48">
         <f>COUNTIF(H7:H46, "Yes")</f>
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3">
@@ -13603,7 +13625,7 @@
       </c>
       <c r="J3" s="52">
         <f>COUNTIF(H7:H46, "No")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -13624,7 +13646,7 @@
       </c>
       <c r="J4" s="101">
         <f>COUNTIF(I7:I46, "Done")</f>
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
@@ -13715,7 +13737,7 @@
         <v>215</v>
       </c>
       <c r="I8" s="106" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J8" s="66"/>
     </row>
@@ -13739,7 +13761,7 @@
         <v>215</v>
       </c>
       <c r="I9" s="106" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J9" s="66"/>
     </row>
@@ -13783,7 +13805,7 @@
         <v>215</v>
       </c>
       <c r="I11" s="106" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J11" s="66"/>
     </row>
@@ -13807,7 +13829,7 @@
         <v>215</v>
       </c>
       <c r="I12" s="106" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J12" s="66"/>
     </row>
@@ -13831,7 +13853,7 @@
         <v>215</v>
       </c>
       <c r="I13" s="106" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J13" s="66"/>
     </row>
@@ -13857,7 +13879,7 @@
         <v>215</v>
       </c>
       <c r="I14" s="106" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J14" s="107"/>
     </row>
@@ -13867,7 +13889,7 @@
       </c>
       <c r="B15" s="43"/>
       <c r="C15" s="68" t="s">
-        <v>105</v>
+        <v>216</v>
       </c>
       <c r="D15" s="43"/>
       <c r="E15" s="73" t="s">
@@ -13883,7 +13905,7 @@
         <v>215</v>
       </c>
       <c r="I15" s="106" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J15" s="66"/>
     </row>
@@ -13893,7 +13915,7 @@
       </c>
       <c r="B16" s="25"/>
       <c r="C16" s="72" t="s">
-        <v>109</v>
+        <v>217</v>
       </c>
       <c r="D16" s="43"/>
       <c r="E16" s="73" t="s">
@@ -13909,7 +13931,7 @@
         <v>215</v>
       </c>
       <c r="I16" s="106" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J16" s="66"/>
     </row>
@@ -13937,7 +13959,7 @@
         <v>215</v>
       </c>
       <c r="I17" s="106" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J17" s="66"/>
     </row>
@@ -13961,7 +13983,7 @@
         <v>215</v>
       </c>
       <c r="I18" s="106" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J18" s="108"/>
     </row>
@@ -14001,13 +14023,15 @@
       <c r="G20" s="68" t="s">
         <v>124</v>
       </c>
-      <c r="H20" s="66" t="s">
-        <v>215</v>
+      <c r="H20" s="68" t="s">
+        <v>59</v>
       </c>
       <c r="I20" s="106" t="s">
-        <v>216</v>
-      </c>
-      <c r="J20" s="66"/>
+        <v>15</v>
+      </c>
+      <c r="J20" s="68" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="63" t="s">
@@ -14049,7 +14073,7 @@
         <v>215</v>
       </c>
       <c r="I22" s="106" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J22" s="66"/>
     </row>
@@ -14093,7 +14117,7 @@
         <v>215</v>
       </c>
       <c r="I24" s="106" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J24" s="66"/>
     </row>
@@ -14121,7 +14145,7 @@
         <v>215</v>
       </c>
       <c r="I25" s="106" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J25" s="66"/>
     </row>
@@ -14161,13 +14185,15 @@
       <c r="G27" s="72" t="s">
         <v>141</v>
       </c>
-      <c r="H27" s="66" t="s">
-        <v>215</v>
+      <c r="H27" s="68" t="s">
+        <v>59</v>
       </c>
       <c r="I27" s="106" t="s">
-        <v>216</v>
-      </c>
-      <c r="J27" s="66"/>
+        <v>15</v>
+      </c>
+      <c r="J27" s="68" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="68" t="s">
@@ -14185,13 +14211,15 @@
       <c r="G28" s="73" t="s">
         <v>145</v>
       </c>
-      <c r="H28" s="66" t="s">
-        <v>215</v>
+      <c r="H28" s="68" t="s">
+        <v>59</v>
       </c>
       <c r="I28" s="106" t="s">
-        <v>216</v>
-      </c>
-      <c r="J28" s="66"/>
+        <v>15</v>
+      </c>
+      <c r="J28" s="68" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="68" t="s">
@@ -14209,13 +14237,15 @@
       <c r="G29" s="72" t="s">
         <v>149</v>
       </c>
-      <c r="H29" s="66" t="s">
-        <v>215</v>
+      <c r="H29" s="68" t="s">
+        <v>59</v>
       </c>
       <c r="I29" s="106" t="s">
-        <v>216</v>
-      </c>
-      <c r="J29" s="66"/>
+        <v>15</v>
+      </c>
+      <c r="J29" s="68" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="68" t="s">
@@ -14233,13 +14263,15 @@
       <c r="G30" s="73" t="s">
         <v>153</v>
       </c>
-      <c r="H30" s="66" t="s">
-        <v>215</v>
+      <c r="H30" s="68" t="s">
+        <v>59</v>
       </c>
       <c r="I30" s="106" t="s">
-        <v>216</v>
-      </c>
-      <c r="J30" s="66"/>
+        <v>15</v>
+      </c>
+      <c r="J30" s="68" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="63" t="s">
@@ -14281,7 +14313,7 @@
         <v>215</v>
       </c>
       <c r="I32" s="106" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J32" s="66"/>
     </row>
@@ -14305,7 +14337,7 @@
         <v>215</v>
       </c>
       <c r="I33" s="106" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J33" s="66"/>
     </row>
@@ -14329,7 +14361,7 @@
         <v>215</v>
       </c>
       <c r="I34" s="106" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J34" s="107"/>
     </row>
@@ -14353,7 +14385,7 @@
         <v>215</v>
       </c>
       <c r="I35" s="106" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J35" s="66"/>
     </row>
@@ -14397,7 +14429,7 @@
         <v>215</v>
       </c>
       <c r="I37" s="106" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J37" s="107"/>
     </row>
@@ -14423,7 +14455,7 @@
         <v>215</v>
       </c>
       <c r="I38" s="106" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J38" s="66"/>
     </row>
@@ -14449,7 +14481,7 @@
         <v>215</v>
       </c>
       <c r="I39" s="106" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J39" s="66"/>
     </row>
@@ -14493,7 +14525,7 @@
         <v>215</v>
       </c>
       <c r="I41" s="106" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J41" s="107"/>
     </row>
@@ -14519,7 +14551,7 @@
         <v>215</v>
       </c>
       <c r="I42" s="106" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J42" s="80"/>
     </row>
@@ -14563,7 +14595,7 @@
         <v>215</v>
       </c>
       <c r="I44" s="106" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J44" s="107"/>
     </row>
@@ -14607,45 +14639,45 @@
         <v>215</v>
       </c>
       <c r="I46" s="106" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J46" s="107"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D11:D18"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="A7:J7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="F8:F9"/>
     <mergeCell ref="A10:J10"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B11:B16"/>
+    <mergeCell ref="D11:D18"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="A19:J19"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="F32:F35"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="F37:F39"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="F41:F42"/>
     <mergeCell ref="A36:J36"/>
     <mergeCell ref="A40:J40"/>
     <mergeCell ref="A43:J43"/>
     <mergeCell ref="A45:J45"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="A19:J19"/>
     <mergeCell ref="A21:J21"/>
     <mergeCell ref="A23:J23"/>
+    <mergeCell ref="B24:B25"/>
     <mergeCell ref="A26:J26"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="F27:F30"/>
     <mergeCell ref="A31:J31"/>
-    <mergeCell ref="F32:F35"/>
-    <mergeCell ref="D32:D35"/>
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B11:B16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="F37:F39"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="B24:B25"/>
   </mergeCells>
   <conditionalFormatting sqref="J2">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
@@ -14727,12 +14759,20 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="I20 I27:I30">
+    <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
+      <formula>"N/A"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="I8:I9 I11:I18 I20 I22 I24:I25 I27:I30 I32:I35 I37:I39 I41:I42 I44 I46">
+    <dataValidation type="list" allowBlank="1" sqref="I8:I9 I11:I18 I22 I24:I25 I32:I35 I37:I39 I41:I42 I44 I46">
       <formula1>"Done,WIP,Select"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="H8:H9 H11:H18 H20 H22 H24:H25 H27:H30 H32:H35 H37:H39 H41:H42 H44 H46">
       <formula1>"Yes,No,Select"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="I20 I27:I30">
+      <formula1>"Done,WIP,Select,N/A"</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions/>
@@ -14772,13 +14812,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="109" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C1" s="39" t="s">
         <v>50</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E1" s="110"/>
       <c r="F1" s="111"/>
@@ -14836,7 +14876,7 @@
         <v>66</v>
       </c>
       <c r="B4" s="112" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C4" s="51"/>
       <c r="D4" s="51"/>
@@ -14886,7 +14926,7 @@
     </row>
     <row r="6">
       <c r="A6" s="115" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B6" s="64"/>
       <c r="C6" s="64"/>
@@ -14958,17 +14998,17 @@
       </c>
       <c r="B9" s="25"/>
       <c r="C9" s="66" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D9" s="75"/>
       <c r="E9" s="66" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="F9" s="66" t="s">
         <v>15</v>
       </c>
       <c r="G9" s="66" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="H9" s="116" t="s">
         <v>215</v>
@@ -14980,7 +15020,7 @@
     </row>
     <row r="10">
       <c r="A10" s="115" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B10" s="64"/>
       <c r="C10" s="64"/>
@@ -15000,19 +15040,19 @@
         <v>16</v>
       </c>
       <c r="C11" s="66" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D11" s="66" t="s">
         <v>80</v>
       </c>
       <c r="E11" s="90" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="F11" s="66" t="s">
         <v>15</v>
       </c>
       <c r="G11" s="90" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H11" s="116" t="s">
         <v>215</v>
@@ -15028,19 +15068,19 @@
       </c>
       <c r="B12" s="43"/>
       <c r="C12" s="66" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="D12" s="66" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="E12" s="89" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="F12" s="66" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="G12" s="89" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="H12" s="116" t="s">
         <v>215</v>
@@ -15056,31 +15096,31 @@
       </c>
       <c r="B13" s="25"/>
       <c r="C13" s="66" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D13" s="66" t="s">
         <v>80</v>
       </c>
       <c r="E13" s="89" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="F13" s="66" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="G13" s="90" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H13" s="116" t="s">
         <v>59</v>
       </c>
       <c r="I13" s="117" t="s">
-        <v>216</v>
+        <v>238</v>
       </c>
       <c r="J13" s="66"/>
     </row>
     <row r="14">
       <c r="A14" s="115" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B14" s="64"/>
       <c r="C14" s="64"/>
@@ -15100,19 +15140,19 @@
         <v>19</v>
       </c>
       <c r="C15" s="66" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="D15" s="66" t="s">
         <v>80</v>
       </c>
       <c r="E15" s="90" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="F15" s="66" t="s">
         <v>15</v>
       </c>
       <c r="G15" s="66" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="H15" s="116" t="s">
         <v>215</v>
@@ -15130,19 +15170,19 @@
         <v>24</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="D16" s="67" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E16" s="90" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="F16" s="67" t="s">
         <v>15</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="H16" s="116" t="s">
         <v>215</v>
@@ -15160,15 +15200,15 @@
         <v>27</v>
       </c>
       <c r="C17" s="66" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="D17" s="43"/>
       <c r="E17" s="66" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="F17" s="43"/>
       <c r="G17" s="66" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="H17" s="116" t="s">
         <v>215</v>
@@ -15186,15 +15226,15 @@
         <v>21</v>
       </c>
       <c r="C18" s="90" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="D18" s="25"/>
       <c r="E18" s="90" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="F18" s="25"/>
       <c r="G18" s="66" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="H18" s="116" t="s">
         <v>215</v>
@@ -15206,7 +15246,7 @@
     </row>
     <row r="19">
       <c r="A19" s="115" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B19" s="64"/>
       <c r="C19" s="64"/>
@@ -15226,19 +15266,19 @@
         <v>30</v>
       </c>
       <c r="C20" s="66" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="D20" s="67" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E20" s="67" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="F20" s="66" t="s">
         <v>15</v>
       </c>
       <c r="G20" s="66" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="H20" s="116" t="s">
         <v>215</v>
@@ -15254,19 +15294,19 @@
       </c>
       <c r="B21" s="43"/>
       <c r="C21" s="66" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="D21" s="67" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E21" s="67" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="F21" s="66" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="G21" s="66" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="H21" s="116" t="s">
         <v>215</v>
@@ -15282,19 +15322,19 @@
       </c>
       <c r="B22" s="25"/>
       <c r="C22" s="66" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="D22" s="67" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E22" s="67" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="F22" s="66" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="G22" s="66" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="H22" s="116" t="s">
         <v>215</v>
@@ -15312,19 +15352,19 @@
         <v>33</v>
       </c>
       <c r="C23" s="66" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D23" s="67" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E23" s="67" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="F23" s="66" t="s">
         <v>15</v>
       </c>
       <c r="G23" s="66" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="H23" s="116" t="s">
         <v>215</v>
@@ -15340,19 +15380,19 @@
       </c>
       <c r="B24" s="43"/>
       <c r="C24" s="66" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="D24" s="67" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E24" s="67" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="F24" s="66" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="G24" s="66" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="H24" s="116" t="s">
         <v>215</v>
@@ -15368,19 +15408,19 @@
       </c>
       <c r="B25" s="25"/>
       <c r="C25" s="66" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="D25" s="67" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E25" s="67" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="F25" s="66" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="G25" s="66" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="H25" s="116" t="s">
         <v>215</v>
@@ -15392,7 +15432,7 @@
     </row>
     <row r="26">
       <c r="A26" s="115" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B26" s="64"/>
       <c r="C26" s="64"/>
@@ -15412,19 +15452,19 @@
         <v>36</v>
       </c>
       <c r="C27" s="66" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="D27" s="67" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E27" s="67" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="F27" s="67" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="G27" s="89" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="H27" s="116" t="s">
         <v>215</v>
@@ -15440,17 +15480,17 @@
       </c>
       <c r="B28" s="43"/>
       <c r="C28" s="66" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="D28" s="67" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E28" s="67" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="F28" s="43"/>
       <c r="G28" s="90" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="H28" s="116" t="s">
         <v>215</v>
@@ -15466,17 +15506,17 @@
       </c>
       <c r="B29" s="43"/>
       <c r="C29" s="66" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="D29" s="67" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E29" s="67" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="F29" s="43"/>
       <c r="G29" s="90" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="H29" s="116" t="s">
         <v>215</v>
@@ -15492,17 +15532,17 @@
       </c>
       <c r="B30" s="25"/>
       <c r="C30" s="66" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="D30" s="67" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E30" s="67" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="F30" s="25"/>
       <c r="G30" s="90" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="H30" s="116" t="s">
         <v>215</v>
@@ -15514,7 +15554,7 @@
     </row>
     <row r="31">
       <c r="A31" s="115" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="B31" s="64"/>
       <c r="C31" s="64"/>
@@ -15534,19 +15574,19 @@
         <v>39</v>
       </c>
       <c r="C32" s="66" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="D32" s="67" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E32" s="67" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="F32" s="66" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="G32" s="66" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="H32" s="116" t="s">
         <v>215</v>
@@ -15564,19 +15604,19 @@
         <v>42</v>
       </c>
       <c r="C33" s="66" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="D33" s="67" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E33" s="67" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="F33" s="66" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="G33" s="66" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="H33" s="116" t="s">
         <v>215</v>
@@ -15588,7 +15628,7 @@
     </row>
     <row r="34">
       <c r="A34" s="115" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="B34" s="64"/>
       <c r="C34" s="64"/>
@@ -15608,19 +15648,19 @@
         <v>45</v>
       </c>
       <c r="C35" s="66" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="D35" s="67" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E35" s="67" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="F35" s="66" t="s">
         <v>15</v>
       </c>
       <c r="G35" s="66" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="H35" s="116" t="s">
         <v>215</v>
@@ -15635,22 +15675,22 @@
         <v>174</v>
       </c>
       <c r="B36" s="66" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C36" s="66" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="D36" s="67" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E36" s="67" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="F36" s="66" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="G36" s="66" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="H36" s="116" t="s">
         <v>215</v>
@@ -15662,7 +15702,7 @@
     </row>
     <row r="37">
       <c r="A37" s="115" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="B37" s="64"/>
       <c r="C37" s="64"/>
@@ -15679,22 +15719,22 @@
         <v>178</v>
       </c>
       <c r="B38" s="66" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="C38" s="90" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="D38" s="67" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E38" s="67" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="F38" s="66" t="s">
         <v>15</v>
       </c>
       <c r="G38" s="66" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="H38" s="116" t="s">
         <v>215</v>
@@ -15709,22 +15749,22 @@
         <v>182</v>
       </c>
       <c r="B39" s="67" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="C39" s="90" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D39" s="67" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E39" s="67" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F39" s="66" t="s">
         <v>15</v>
       </c>
       <c r="G39" s="66" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="H39" s="116" t="s">
         <v>215</v>
@@ -15740,19 +15780,19 @@
       </c>
       <c r="B40" s="43"/>
       <c r="C40" s="90" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="D40" s="67" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E40" s="67" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="F40" s="66" t="s">
         <v>15</v>
       </c>
       <c r="G40" s="66" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="H40" s="116" t="s">
         <v>215</v>
@@ -15764,7 +15804,7 @@
     </row>
     <row r="41">
       <c r="A41" s="115" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="B41" s="64"/>
       <c r="C41" s="64"/>
@@ -15781,22 +15821,22 @@
         <v>190</v>
       </c>
       <c r="B42" s="67" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C42" s="66" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="D42" s="66" t="s">
         <v>80</v>
       </c>
       <c r="E42" s="67" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="F42" s="66" t="s">
         <v>15</v>
       </c>
       <c r="G42" s="66" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="H42" s="116" t="s">
         <v>215</v>
@@ -15812,19 +15852,19 @@
       </c>
       <c r="B43" s="43"/>
       <c r="C43" s="66" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="D43" s="66" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="E43" s="67" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="F43" s="66" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="G43" s="66" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="H43" s="116" t="s">
         <v>215</v>
@@ -15836,7 +15876,7 @@
     </row>
     <row r="44">
       <c r="A44" s="115" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="B44" s="64"/>
       <c r="C44" s="64"/>
@@ -15850,37 +15890,37 @@
     </row>
     <row r="45">
       <c r="A45" s="66" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="B45" s="66" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="C45" s="66" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="D45" s="66" t="s">
         <v>80</v>
       </c>
       <c r="E45" s="66" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="F45" s="66" t="s">
         <v>15</v>
       </c>
       <c r="G45" s="66" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="H45" s="116" t="s">
         <v>59</v>
       </c>
       <c r="I45" s="117" t="s">
-        <v>216</v>
+        <v>238</v>
       </c>
       <c r="J45" s="66"/>
     </row>
     <row r="46">
       <c r="A46" s="119" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="B46" s="82"/>
       <c r="C46" s="82"/>
@@ -15894,37 +15934,37 @@
     </row>
     <row r="47">
       <c r="A47" s="120" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="B47" s="121" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="C47" s="112" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="D47" s="112" t="s">
         <v>80</v>
       </c>
       <c r="E47" s="112" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="F47" s="112" t="s">
         <v>15</v>
       </c>
       <c r="G47" s="112" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="H47" s="116" t="s">
         <v>59</v>
       </c>
       <c r="I47" s="117" t="s">
-        <v>216</v>
+        <v>238</v>
       </c>
       <c r="J47" s="86"/>
     </row>
     <row r="48">
       <c r="A48" s="119" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="B48" s="82"/>
       <c r="C48" s="82"/>
@@ -15938,57 +15978,57 @@
     </row>
     <row r="49">
       <c r="A49" s="120" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="B49" s="122" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="C49" s="112" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="D49" s="123" t="s">
         <v>80</v>
       </c>
       <c r="E49" s="112" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="F49" s="112" t="s">
         <v>15</v>
       </c>
       <c r="G49" s="112" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="H49" s="116" t="s">
         <v>59</v>
       </c>
       <c r="I49" s="117" t="s">
-        <v>216</v>
+        <v>238</v>
       </c>
       <c r="J49" s="86"/>
     </row>
     <row r="50">
       <c r="A50" s="120" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="B50" s="65"/>
       <c r="C50" s="66" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="D50" s="65"/>
       <c r="E50" s="112" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="F50" s="112" t="s">
         <v>15</v>
       </c>
       <c r="G50" s="66" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="H50" s="116" t="s">
         <v>59</v>
       </c>
       <c r="I50" s="117" t="s">
-        <v>216</v>
+        <v>238</v>
       </c>
       <c r="J50" s="66"/>
     </row>
@@ -18549,35 +18589,35 @@
     <row r="911" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="A26:J26"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B27:B30"/>
     <mergeCell ref="F27:F30"/>
-    <mergeCell ref="A48:J48"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="A41:J41"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A19:J19"/>
-    <mergeCell ref="A44:J44"/>
-    <mergeCell ref="A46:J46"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="A14:J14"/>
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A10:J10"/>
-    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="I1:J1"/>
     <mergeCell ref="A6:J6"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="F7:F8"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="A10:J10"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="A44:J44"/>
+    <mergeCell ref="A46:J46"/>
+    <mergeCell ref="A48:J48"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="A14:J14"/>
+    <mergeCell ref="A19:J19"/>
+    <mergeCell ref="A26:J26"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="A34:J34"/>
     <mergeCell ref="A37:J37"/>
-    <mergeCell ref="A34:J34"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A41:J41"/>
   </mergeCells>
   <conditionalFormatting sqref="J2">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
@@ -18719,7 +18759,7 @@
     <row r="2">
       <c r="A2" s="128"/>
       <c r="B2" s="129" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C2" s="82"/>
       <c r="D2" s="82"/>
@@ -18749,7 +18789,7 @@
     <row r="3">
       <c r="A3" s="128"/>
       <c r="B3" s="130" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="C3" s="82"/>
       <c r="D3" s="82"/>
@@ -18779,19 +18819,19 @@
     <row r="4">
       <c r="A4" s="128"/>
       <c r="B4" s="131" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="C4" s="131" t="s">
         <v>68</v>
       </c>
       <c r="D4" s="131" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="E4" s="131" t="s">
         <v>210</v>
       </c>
       <c r="F4" s="131" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="G4" s="128"/>
       <c r="H4" s="128"/>
@@ -18826,12 +18866,11 @@
       <c r="D5" s="132">
         <v>0.0</v>
       </c>
-      <c r="E5" s="132">
-        <f>COUNTA(TestCase_and_TestExecution!C8:C9)</f>
-        <v>2</v>
+      <c r="E5" s="133">
+        <v>2.0</v>
       </c>
       <c r="F5" s="132" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G5" s="128"/>
       <c r="H5" s="128"/>
@@ -18856,7 +18895,7 @@
     </row>
     <row r="6">
       <c r="A6" s="128"/>
-      <c r="B6" s="133" t="s">
+      <c r="B6" s="134" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="132">
@@ -18866,12 +18905,11 @@
       <c r="D6" s="132">
         <v>0.0</v>
       </c>
-      <c r="E6" s="132">
-        <f>COUNTA(TestCase_and_TestExecution!C11:C18)</f>
-        <v>8</v>
+      <c r="E6" s="133">
+        <v>8.0</v>
       </c>
       <c r="F6" s="132" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G6" s="128"/>
       <c r="H6" s="128"/>
@@ -18903,15 +18941,14 @@
         <f>COUNTA(TestCase_and_TestExecution!A20)</f>
         <v>1</v>
       </c>
-      <c r="D7" s="132">
+      <c r="D7" s="133">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="133">
         <v>0.0</v>
       </c>
-      <c r="E7" s="132">
-        <f>COUNTA(TestCase_and_TestExecution!C20)</f>
-        <v>1</v>
-      </c>
       <c r="F7" s="132" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G7" s="128"/>
       <c r="H7" s="128"/>
@@ -18946,12 +18983,11 @@
       <c r="D8" s="132">
         <v>0.0</v>
       </c>
-      <c r="E8" s="132">
-        <f>COUNTA(TestCase_and_TestExecution!C22)</f>
-        <v>1</v>
+      <c r="E8" s="133">
+        <v>1.0</v>
       </c>
       <c r="F8" s="132" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G8" s="128"/>
       <c r="H8" s="128"/>
@@ -18986,12 +19022,11 @@
       <c r="D9" s="132">
         <v>0.0</v>
       </c>
-      <c r="E9" s="132">
-        <f>COUNTA(TestCase_and_TestExecution!C24:C25)</f>
-        <v>2</v>
+      <c r="E9" s="133">
+        <v>2.0</v>
       </c>
       <c r="F9" s="132" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G9" s="128"/>
       <c r="H9" s="128"/>
@@ -19023,15 +19058,14 @@
         <f>COUNTA(TestCase_and_TestExecution!A27:A30)</f>
         <v>4</v>
       </c>
-      <c r="D10" s="132">
+      <c r="D10" s="133">
+        <v>4.0</v>
+      </c>
+      <c r="E10" s="133">
         <v>0.0</v>
       </c>
-      <c r="E10" s="132">
-        <f>COUNTA(TestCase_and_TestExecution!C27:C30)</f>
-        <v>4</v>
-      </c>
       <c r="F10" s="132" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G10" s="128"/>
       <c r="H10" s="128"/>
@@ -19066,12 +19100,11 @@
       <c r="D11" s="132">
         <v>0.0</v>
       </c>
-      <c r="E11" s="132">
-        <f>COUNTA(TestCase_and_TestExecution!C32:C35)</f>
-        <v>4</v>
+      <c r="E11" s="133">
+        <v>4.0</v>
       </c>
       <c r="F11" s="132" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G11" s="128"/>
       <c r="H11" s="128"/>
@@ -19106,12 +19139,11 @@
       <c r="D12" s="132">
         <v>0.0</v>
       </c>
-      <c r="E12" s="132">
-        <f>COUNTA(TestCase_and_TestExecution!C37:C39)</f>
-        <v>3</v>
+      <c r="E12" s="133">
+        <v>3.0</v>
       </c>
       <c r="F12" s="132" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G12" s="128"/>
       <c r="H12" s="128"/>
@@ -19146,12 +19178,11 @@
       <c r="D13" s="132">
         <v>0.0</v>
       </c>
-      <c r="E13" s="132">
-        <f>COUNTA(TestCase_and_TestExecution!C41:C42)</f>
-        <v>2</v>
+      <c r="E13" s="133">
+        <v>2.0</v>
       </c>
       <c r="F13" s="132" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G13" s="128"/>
       <c r="H13" s="128"/>
@@ -19175,7 +19206,7 @@
       <c r="Z13" s="128"/>
     </row>
     <row r="14">
-      <c r="A14" s="134"/>
+      <c r="A14" s="135"/>
       <c r="B14" s="28" t="s">
         <v>43</v>
       </c>
@@ -19186,33 +19217,32 @@
       <c r="D14" s="132">
         <v>0.0</v>
       </c>
-      <c r="E14" s="132">
-        <f>COUNTA(TestCase_and_TestExecution!C44)</f>
-        <v>1</v>
-      </c>
-      <c r="F14" s="135" t="s">
-        <v>351</v>
-      </c>
-      <c r="G14" s="134"/>
-      <c r="H14" s="134"/>
-      <c r="I14" s="134"/>
-      <c r="J14" s="134"/>
-      <c r="K14" s="136"/>
-      <c r="L14" s="134"/>
-      <c r="M14" s="134"/>
-      <c r="N14" s="134"/>
-      <c r="O14" s="134"/>
-      <c r="P14" s="134"/>
-      <c r="Q14" s="134"/>
-      <c r="R14" s="134"/>
-      <c r="S14" s="134"/>
-      <c r="T14" s="134"/>
-      <c r="U14" s="134"/>
-      <c r="V14" s="134"/>
-      <c r="W14" s="134"/>
-      <c r="X14" s="134"/>
-      <c r="Y14" s="134"/>
-      <c r="Z14" s="134"/>
+      <c r="E14" s="133">
+        <v>1.0</v>
+      </c>
+      <c r="F14" s="136" t="s">
+        <v>354</v>
+      </c>
+      <c r="G14" s="135"/>
+      <c r="H14" s="135"/>
+      <c r="I14" s="135"/>
+      <c r="J14" s="135"/>
+      <c r="K14" s="137"/>
+      <c r="L14" s="135"/>
+      <c r="M14" s="135"/>
+      <c r="N14" s="135"/>
+      <c r="O14" s="135"/>
+      <c r="P14" s="135"/>
+      <c r="Q14" s="135"/>
+      <c r="R14" s="135"/>
+      <c r="S14" s="135"/>
+      <c r="T14" s="135"/>
+      <c r="U14" s="135"/>
+      <c r="V14" s="135"/>
+      <c r="W14" s="135"/>
+      <c r="X14" s="135"/>
+      <c r="Y14" s="135"/>
+      <c r="Z14" s="135"/>
     </row>
     <row r="15">
       <c r="A15" s="128"/>
@@ -19226,18 +19256,17 @@
       <c r="D15" s="132">
         <v>0.0</v>
       </c>
-      <c r="E15" s="132">
-        <f>COUNTA(TestCase_and_TestExecution!C44)</f>
-        <v>1</v>
+      <c r="E15" s="133">
+        <v>1.0</v>
       </c>
       <c r="F15" s="132" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G15" s="128"/>
       <c r="H15" s="128"/>
       <c r="I15" s="128"/>
       <c r="J15" s="128"/>
-      <c r="K15" s="137"/>
+      <c r="K15" s="138"/>
       <c r="L15" s="128"/>
       <c r="M15" s="128"/>
       <c r="N15" s="128"/>
@@ -19256,27 +19285,27 @@
     </row>
     <row r="16">
       <c r="A16" s="128"/>
-      <c r="B16" s="138" t="s">
+      <c r="B16" s="139" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="138">
+      <c r="C16" s="139">
         <f>SUM(C5:C15)</f>
         <v>29</v>
       </c>
-      <c r="D16" s="138">
+      <c r="D16" s="139">
         <f t="shared" ref="D16:E16" si="1">sum(D5:D15)</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="138">
+        <v>5</v>
+      </c>
+      <c r="E16" s="139">
         <f t="shared" si="1"/>
-        <v>29</v>
-      </c>
-      <c r="F16" s="138"/>
+        <v>24</v>
+      </c>
+      <c r="F16" s="139"/>
       <c r="G16" s="128"/>
       <c r="H16" s="128"/>
       <c r="I16" s="128"/>
       <c r="J16" s="128"/>
-      <c r="K16" s="137"/>
+      <c r="K16" s="138"/>
       <c r="L16" s="128"/>
       <c r="M16" s="128"/>
       <c r="N16" s="128"/>
@@ -19377,11 +19406,11 @@
     <row r="20">
       <c r="A20" s="128"/>
       <c r="B20" s="129" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C20" s="42"/>
-      <c r="D20" s="139"/>
-      <c r="E20" s="139"/>
+      <c r="D20" s="140"/>
+      <c r="E20" s="140"/>
       <c r="F20" s="128"/>
       <c r="G20" s="128"/>
       <c r="H20" s="128"/>
@@ -19405,14 +19434,14 @@
     </row>
     <row r="21">
       <c r="A21" s="128"/>
-      <c r="B21" s="140" t="s">
-        <v>353</v>
-      </c>
-      <c r="C21" s="140" t="s">
-        <v>354</v>
-      </c>
-      <c r="D21" s="139"/>
-      <c r="E21" s="139"/>
+      <c r="B21" s="141" t="s">
+        <v>356</v>
+      </c>
+      <c r="C21" s="141" t="s">
+        <v>357</v>
+      </c>
+      <c r="D21" s="140"/>
+      <c r="E21" s="140"/>
       <c r="F21" s="128"/>
       <c r="G21" s="128"/>
       <c r="H21" s="128"/>
@@ -19436,14 +19465,14 @@
     </row>
     <row r="22">
       <c r="A22" s="128"/>
-      <c r="B22" s="141" t="s">
-        <v>355</v>
-      </c>
-      <c r="C22" s="142" t="s">
-        <v>356</v>
-      </c>
-      <c r="D22" s="139"/>
-      <c r="E22" s="139"/>
+      <c r="B22" s="142" t="s">
+        <v>358</v>
+      </c>
+      <c r="C22" s="143" t="s">
+        <v>359</v>
+      </c>
+      <c r="D22" s="140"/>
+      <c r="E22" s="140"/>
       <c r="F22" s="128"/>
       <c r="G22" s="128"/>
       <c r="H22" s="128"/>
@@ -19467,15 +19496,15 @@
     </row>
     <row r="23">
       <c r="A23" s="128"/>
-      <c r="B23" s="141" t="s">
-        <v>357</v>
+      <c r="B23" s="142" t="s">
+        <v>360</v>
       </c>
       <c r="C23" s="132">
         <f>C16</f>
         <v>29</v>
       </c>
-      <c r="D23" s="139"/>
-      <c r="E23" s="139"/>
+      <c r="D23" s="140"/>
+      <c r="E23" s="140"/>
       <c r="F23" s="128"/>
       <c r="G23" s="128"/>
       <c r="H23" s="128"/>
@@ -19500,15 +19529,15 @@
     </row>
     <row r="24">
       <c r="A24" s="128"/>
-      <c r="B24" s="141" t="s">
+      <c r="B24" s="142" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="135">
+      <c r="C24" s="136">
         <f>COUNTIF(TestCase_and_TestExecution!I8:I46,"PASS")</f>
         <v>29</v>
       </c>
-      <c r="D24" s="139"/>
-      <c r="E24" s="139"/>
+      <c r="D24" s="140"/>
+      <c r="E24" s="140"/>
       <c r="F24" s="128"/>
       <c r="G24" s="128"/>
       <c r="H24" s="128"/>
@@ -19533,15 +19562,15 @@
     </row>
     <row r="25">
       <c r="A25" s="128"/>
-      <c r="B25" s="141" t="s">
-        <v>358</v>
+      <c r="B25" s="142" t="s">
+        <v>361</v>
       </c>
       <c r="C25" s="132">
         <f>COUNTIF(TestCase_and_TestExecution!I8:I46,"FAIL")</f>
         <v>0</v>
       </c>
-      <c r="D25" s="139"/>
-      <c r="E25" s="139"/>
+      <c r="D25" s="140"/>
+      <c r="E25" s="140"/>
       <c r="F25" s="128"/>
       <c r="G25" s="128"/>
       <c r="H25" s="128"/>
@@ -19566,15 +19595,15 @@
     </row>
     <row r="26">
       <c r="A26" s="128"/>
-      <c r="B26" s="141" t="s">
+      <c r="B26" s="142" t="s">
         <v>64</v>
       </c>
       <c r="C26" s="132">
         <f>COUNTIF(TestCase_and_TestExecution!I8:I46,"WARNING")</f>
         <v>0</v>
       </c>
-      <c r="D26" s="139"/>
-      <c r="E26" s="139"/>
+      <c r="D26" s="140"/>
+      <c r="E26" s="140"/>
       <c r="F26" s="128"/>
       <c r="G26" s="128"/>
       <c r="H26" s="128"/>
@@ -19599,15 +19628,15 @@
     </row>
     <row r="27">
       <c r="A27" s="128"/>
-      <c r="B27" s="141" t="s">
-        <v>359</v>
+      <c r="B27" s="142" t="s">
+        <v>362</v>
       </c>
       <c r="C27" s="132">
         <f>COUNTIF(TestCase_and_TestExecution!I8:I46,"N/T")</f>
         <v>0</v>
       </c>
-      <c r="D27" s="139"/>
-      <c r="E27" s="139"/>
+      <c r="D27" s="140"/>
+      <c r="E27" s="140"/>
       <c r="F27" s="128"/>
       <c r="G27" s="128"/>
       <c r="H27" s="128"/>
@@ -19632,15 +19661,15 @@
     </row>
     <row r="28">
       <c r="A28" s="128"/>
-      <c r="B28" s="141" t="s">
-        <v>360</v>
+      <c r="B28" s="142" t="s">
+        <v>363</v>
       </c>
       <c r="C28" s="132">
         <f>COUNTIF(TestCase_and_TestExecution!I8:I46,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="D28" s="139"/>
-      <c r="E28" s="139"/>
+      <c r="D28" s="140"/>
+      <c r="E28" s="140"/>
       <c r="F28" s="128"/>
       <c r="G28" s="128"/>
       <c r="H28" s="128"/>
@@ -19665,15 +19694,15 @@
     </row>
     <row r="29">
       <c r="A29" s="128"/>
-      <c r="B29" s="141" t="s">
-        <v>361</v>
+      <c r="B29" s="142" t="s">
+        <v>364</v>
       </c>
       <c r="C29" s="132">
         <f>COUNTIF(TestCase_and_TestExecution!I8:I46,"WIP")</f>
         <v>0</v>
       </c>
-      <c r="D29" s="139"/>
-      <c r="E29" s="139"/>
+      <c r="D29" s="140"/>
+      <c r="E29" s="140"/>
       <c r="F29" s="128"/>
       <c r="G29" s="128"/>
       <c r="H29" s="128"/>
@@ -19698,15 +19727,15 @@
     </row>
     <row r="30">
       <c r="A30" s="128"/>
-      <c r="B30" s="138" t="s">
-        <v>362</v>
-      </c>
-      <c r="C30" s="143">
+      <c r="B30" s="139" t="s">
+        <v>365</v>
+      </c>
+      <c r="C30" s="144">
         <f>C24/(C23-C27-C28-C29)</f>
         <v>1</v>
       </c>
-      <c r="D30" s="139"/>
-      <c r="E30" s="139"/>
+      <c r="D30" s="140"/>
+      <c r="E30" s="140"/>
       <c r="F30" s="128"/>
       <c r="G30" s="128"/>
       <c r="H30" s="128"/>
@@ -19733,8 +19762,8 @@
       <c r="A31" s="128"/>
       <c r="B31" s="128"/>
       <c r="C31" s="128"/>
-      <c r="D31" s="139"/>
-      <c r="E31" s="139"/>
+      <c r="D31" s="140"/>
+      <c r="E31" s="140"/>
       <c r="F31" s="128"/>
       <c r="G31" s="128"/>
       <c r="H31" s="128"/>
@@ -19761,8 +19790,8 @@
       <c r="A32" s="128"/>
       <c r="B32" s="128"/>
       <c r="C32" s="128"/>
-      <c r="D32" s="139"/>
-      <c r="E32" s="139"/>
+      <c r="D32" s="140"/>
+      <c r="E32" s="140"/>
       <c r="F32" s="128"/>
       <c r="G32" s="128"/>
       <c r="H32" s="128"/>
@@ -19789,8 +19818,8 @@
       <c r="A33" s="128"/>
       <c r="B33" s="128"/>
       <c r="C33" s="128"/>
-      <c r="D33" s="139"/>
-      <c r="E33" s="139"/>
+      <c r="D33" s="140"/>
+      <c r="E33" s="140"/>
       <c r="F33" s="128"/>
       <c r="G33" s="128"/>
       <c r="H33" s="128"/>

</xml_diff>